<commit_message>
adding back fastq files
</commit_message>
<xml_diff>
--- a/library/library_H.BROWN_11.10.19.xlsx
+++ b/library/library_H.BROWN_11.10.19.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63C04AA-396A-A04F-AD8C-450458DE6E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DC051F-8D6D-BC44-8A5F-73CF8638AB0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="16820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -712,7 +712,7 @@
   <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I41"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2351,6 +2351,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>